<commit_message>
update upload account data
</commit_message>
<xml_diff>
--- a/public/template/uploadAccountData/templateAccountData.xlsx
+++ b/public/template/uploadAccountData/templateAccountData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ecent\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kantor\cms_ci4_v1_2\public\template\uploadAccountData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B100CFD0-F626-4C3B-8CFC-10E9D797B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CF58E4-D751-4BB3-BBD7-0F010ED1FB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{566D570E-E14F-4C35-8CCF-A36E5E96BCB9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1923" uniqueCount="560">
   <si>
     <t>CM_CUSTOMER_NMBR</t>
   </si>
@@ -1688,6 +1688,18 @@
   </si>
   <si>
     <t>03:23.0</t>
+  </si>
+  <si>
+    <t>AGENT_ID</t>
+  </si>
+  <si>
+    <t>CM_BUCKET</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>CURRENT</t>
   </si>
 </sst>
 </file>
@@ -2550,10 +2562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06EB513-77A7-49AF-884C-C90CE79E03E3}">
-  <dimension ref="A1:BU101"/>
+  <dimension ref="A1:BW101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BW3" sqref="BW3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2564,7 +2576,7 @@
     <col min="66" max="66" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2784,8 +2796,14 @@
       <c r="BU1" t="s">
         <v>72</v>
       </c>
+      <c r="BV1" t="s">
+        <v>556</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>557</v>
+      </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2603202498765</v>
       </c>
@@ -2897,8 +2915,14 @@
       <c r="BS2">
         <v>0</v>
       </c>
+      <c r="BV2" t="s">
+        <v>558</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>559</v>
+      </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2603202498765</v>
       </c>
@@ -3014,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2603202498767</v>
       </c>
@@ -3130,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>2603202498768</v>
       </c>
@@ -3246,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2603202498769</v>
       </c>
@@ -3362,7 +3386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>2603202498770</v>
       </c>
@@ -3478,7 +3502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>2603202498771</v>
       </c>
@@ -3594,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>2603202498772</v>
       </c>
@@ -3710,7 +3734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>2603202498773</v>
       </c>
@@ -3823,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>2603202498774</v>
       </c>
@@ -3939,7 +3963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>2603202498775</v>
       </c>
@@ -4055,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>2603202498776</v>
       </c>
@@ -4171,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2603202498777</v>
       </c>
@@ -4287,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2603202498778</v>
       </c>
@@ -4403,7 +4427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:75" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2603202498779</v>
       </c>

</xml_diff>